<commit_message>
Idealização da Documentação do Projeto
</commit_message>
<xml_diff>
--- a/HROADS/Modelagem/hroads_modelagem-Fisico.xlsx
+++ b/HROADS/Modelagem/hroads_modelagem-Fisico.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\livia\OneDrive\Documents\Lívia\Lívia Escola\SENAI\sprint-1-bd\exercicios\Desafio-HROADS\HROADS\Modelagem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilherme_2\Documents\trabalhos do leo\Senai\Desafio-HROADS\HROADS\Modelagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4286A70A-99FB-4992-89CF-58A695629058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB3EF08-6919-4BF7-85BE-68602D5BDEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CFC85692-09BB-4DB3-A9E1-59BB43735922}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{CFC85692-09BB-4DB3-A9E1-59BB43735922}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -355,40 +355,40 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -714,43 +714,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF687E9-ABA7-4743-80C3-9944A936F544}">
   <dimension ref="B2:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.5703125" customWidth="1"/>
     <col min="13" max="13" width="12.140625" customWidth="1"/>
     <col min="14" max="14" width="21.28515625" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" customWidth="1"/>
-    <col min="16" max="16" width="18.5703125" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="E2" s="16" t="s">
+      <c r="C2" s="26"/>
+      <c r="E2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
     </row>
@@ -770,14 +770,14 @@
       <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
     </row>
@@ -797,14 +797,14 @@
       <c r="G4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
     </row>
@@ -824,14 +824,14 @@
       <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
     </row>
@@ -851,14 +851,14 @@
       <c r="G6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
     </row>
@@ -875,24 +875,24 @@
       <c r="H7" s="1"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="F12" s="20" t="s">
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="F12" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
@@ -910,15 +910,15 @@
       <c r="G13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
       <c r="O13" s="3" t="s">
         <v>25</v>
       </c>
@@ -942,15 +942,15 @@
       <c r="G14" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
       <c r="O14" s="3">
         <v>100</v>
       </c>
@@ -974,15 +974,15 @@
       <c r="G15" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
       <c r="O15" s="3">
         <v>80</v>
       </c>
@@ -1006,15 +1006,15 @@
       <c r="G16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="H16" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
       <c r="O16" s="3">
         <v>95</v>
       </c>
@@ -1038,15 +1038,15 @@
       <c r="G17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H17" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
       <c r="O17" s="3">
         <v>70</v>
       </c>
@@ -1070,15 +1070,15 @@
       <c r="G18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H18" s="21" t="s">
+      <c r="H18" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="23"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="18"/>
       <c r="O18" s="3">
         <v>60</v>
       </c>
@@ -1102,15 +1102,15 @@
       <c r="G19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H19" s="21" t="s">
+      <c r="H19" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="23"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="18"/>
       <c r="O19" s="3">
         <v>85</v>
       </c>
@@ -1134,15 +1134,15 @@
       <c r="G20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="23"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="18"/>
       <c r="O20" s="3">
         <v>75</v>
       </c>
@@ -1179,13 +1179,13 @@
       <c r="P22" s="14"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E26" s="24" t="s">
+      <c r="E26" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="26"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="21"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E27" s="3" t="s">
@@ -1257,23 +1257,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H17:N17"/>
-    <mergeCell ref="H18:N18"/>
-    <mergeCell ref="H19:N19"/>
-    <mergeCell ref="H20:N20"/>
-    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="E2:M2"/>
+    <mergeCell ref="H14:N14"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="H4:M4"/>
     <mergeCell ref="H15:N15"/>
     <mergeCell ref="H16:N16"/>
     <mergeCell ref="H13:N13"/>
     <mergeCell ref="F12:P12"/>
     <mergeCell ref="H5:M5"/>
     <mergeCell ref="H6:M6"/>
-    <mergeCell ref="H3:M3"/>
-    <mergeCell ref="E2:M2"/>
-    <mergeCell ref="H14:N14"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="H4:M4"/>
+    <mergeCell ref="H17:N17"/>
+    <mergeCell ref="H18:N18"/>
+    <mergeCell ref="H19:N19"/>
+    <mergeCell ref="H20:N20"/>
+    <mergeCell ref="E26:I26"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>